<commit_message>
Add import script for transactions
</commit_message>
<xml_diff>
--- a/server/transparencyportal/upload/imports/local_test.xlsx
+++ b/server/transparencyportal/upload/imports/local_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Guides" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="336">
   <si>
     <t>Couleur des entêtes</t>
   </si>
@@ -4572,41 +4572,42 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" customWidth="1"/>
-    <col min="8" max="11" width="31.28515625" customWidth="1"/>
-    <col min="12" max="12" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="10" width="31.28515625" customWidth="1"/>
+    <col min="11" max="11" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8"/>
       <c r="B1" s="34" t="s">
         <v>188</v>
       </c>
       <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>189</v>
       </c>
+      <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -4616,8 +4617,8 @@
       <c r="C2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>42</v>
+      <c r="D2" s="24" t="s">
+        <v>149</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>149</v>
@@ -4628,23 +4629,20 @@
       <c r="G2" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H2" s="24" t="s">
-        <v>149</v>
+      <c r="H2" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>148</v>
+      <c r="J2" s="24" t="s">
+        <v>149</v>
       </c>
       <c r="K2" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="L2" s="24" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -4655,34 +4653,31 @@
         <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>193</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>194</v>
+      </c>
       <c r="K3" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="L3" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -4692,33 +4687,30 @@
       <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
-        <v>1</v>
-      </c>
-      <c r="E4" s="25" t="s">
+      <c r="D4" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="E4" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="F4" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25" t="s">
+      <c r="I4" s="25"/>
+      <c r="J4" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -4728,33 +4720,30 @@
       <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="11">
-        <v>2</v>
+      <c r="D5" s="25" t="s">
+        <v>201</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="F5" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25" t="s">
+      <c r="I5" s="25"/>
+      <c r="J5" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -4764,33 +4753,30 @@
       <c r="C6" s="11">
         <v>1</v>
       </c>
-      <c r="D6" s="11">
-        <v>3</v>
+      <c r="D6" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="F6" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="G6" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25" t="s">
+      <c r="I6" s="25"/>
+      <c r="J6" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -4800,33 +4786,30 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="11">
-        <v>4</v>
+      <c r="D7" s="25" t="s">
+        <v>207</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="F7" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="F7" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="G7" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25" t="s">
+      <c r="I7" s="25"/>
+      <c r="J7" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>5</v>
       </c>
@@ -4836,33 +4819,30 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="11">
-        <v>5</v>
+      <c r="D8" s="25" t="s">
+        <v>209</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="F8" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="F8" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="G8" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25" t="s">
+      <c r="I8" s="25"/>
+      <c r="J8" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="K8" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>6</v>
       </c>
@@ -4872,33 +4852,30 @@
       <c r="C9" s="11">
         <v>1</v>
       </c>
-      <c r="D9" s="11">
-        <v>6</v>
+      <c r="D9" s="25" t="s">
+        <v>212</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>212</v>
-      </c>
-      <c r="F9" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="F9" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="G9" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25" t="s">
+      <c r="I9" s="25"/>
+      <c r="J9" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="K9" s="8" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>7</v>
       </c>
@@ -4908,33 +4885,30 @@
       <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="D10" s="11">
-        <v>7</v>
+      <c r="D10" s="25" t="s">
+        <v>215</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="F10" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="F10" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="G10" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25" t="s">
+      <c r="I10" s="25"/>
+      <c r="J10" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>8</v>
       </c>
@@ -4944,33 +4918,30 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="11">
-        <v>8</v>
+      <c r="D11" s="25" t="s">
+        <v>196</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="F11" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="F11" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="G11" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="H11" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25" t="s">
+      <c r="I11" s="25"/>
+      <c r="J11" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="K11" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>9</v>
       </c>
@@ -4980,33 +4951,30 @@
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="11">
-        <v>9</v>
+      <c r="D12" s="25" t="s">
+        <v>218</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="F12" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="F12" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="G12" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="H12" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25" t="s">
+      <c r="I12" s="25"/>
+      <c r="J12" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="K12" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>10</v>
       </c>
@@ -5016,36 +4984,33 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="11">
-        <v>10</v>
+      <c r="D13" s="25" t="s">
+        <v>220</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="F13" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="F13" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="G13" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25" t="s">
+      <c r="I13" s="25"/>
+      <c r="J13" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="K13" s="8" t="s">
         <v>203</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:K1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B4:B13">
@@ -5053,8 +5018,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5064,7 +5029,7 @@
           <x14:formula1>
             <xm:f>Constantes!$O$2:$O$42</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E13</xm:sqref>
+          <xm:sqref>D4:D13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5077,44 +5042,45 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" customWidth="1"/>
-    <col min="6" max="9" width="31.28515625" customWidth="1"/>
-    <col min="11" max="11" width="27.42578125" customWidth="1"/>
-    <col min="12" max="12" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="5" max="8" width="31.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8"/>
       <c r="B1" s="34" t="s">
         <v>188</v>
       </c>
       <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="36" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="36" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J1" s="32"/>
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -5124,23 +5090,23 @@
       <c r="C2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>149</v>
@@ -5148,11 +5114,8 @@
       <c r="K2" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="L2" s="24" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -5163,34 +5126,31 @@
         <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -5200,35 +5160,32 @@
       <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
-        <v>1</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F4" s="22">
+      <c r="E4" s="22">
         <v>10</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H4" s="22">
+      <c r="G4" s="22">
         <v>2500</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="H4" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I4" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J4" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="K4" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="K4" s="19" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -5238,35 +5195,32 @@
       <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="11">
-        <v>2</v>
-      </c>
-      <c r="E5" s="22" t="s">
+      <c r="D5" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F5" s="22">
+      <c r="E5" s="22">
         <v>5</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H5" s="22">
+      <c r="G5" s="22">
         <v>2500</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="H5" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I5" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J5" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L5" s="8" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -5276,35 +5230,32 @@
       <c r="C6" s="11">
         <v>1</v>
       </c>
-      <c r="D6" s="11">
-        <v>3</v>
-      </c>
-      <c r="E6" s="22" t="s">
+      <c r="D6" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F6" s="22">
+      <c r="E6" s="22">
         <v>7</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H6" s="22">
+      <c r="G6" s="22">
         <v>2500</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="H6" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I6" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J6" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L6" s="8" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -5314,35 +5265,32 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="11">
-        <v>4</v>
-      </c>
-      <c r="E7" s="22" t="s">
+      <c r="D7" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F7" s="22">
+      <c r="E7" s="22">
         <v>6</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H7" s="22">
+      <c r="G7" s="22">
         <v>2500</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="H7" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I7" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J7" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L7" s="8" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>5</v>
       </c>
@@ -5352,35 +5300,32 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="22">
         <v>5</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F8" s="22">
-        <v>5</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H8" s="22">
+      <c r="G8" s="22">
         <v>2500</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="H8" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I8" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J8" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L8" s="8" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>6</v>
       </c>
@@ -5390,35 +5335,32 @@
       <c r="C9" s="11">
         <v>1</v>
       </c>
-      <c r="D9" s="11">
-        <v>6</v>
-      </c>
-      <c r="E9" s="22" t="s">
+      <c r="D9" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F9" s="22">
+      <c r="E9" s="22">
         <v>4</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H9" s="22">
+      <c r="G9" s="22">
         <v>2500</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I9" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J9" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L9" s="8" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>7</v>
       </c>
@@ -5428,35 +5370,32 @@
       <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="D10" s="11">
-        <v>7</v>
-      </c>
-      <c r="E10" s="22" t="s">
+      <c r="D10" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F10" s="22">
+      <c r="E10" s="22">
         <v>8</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H10" s="22">
+      <c r="G10" s="22">
         <v>2500</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="H10" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I10" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J10" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L10" s="8" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>8</v>
       </c>
@@ -5466,35 +5405,32 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="11">
-        <v>8</v>
-      </c>
-      <c r="E11" s="22" t="s">
+      <c r="D11" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F11" s="22">
+      <c r="E11" s="22">
         <v>9</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H11" s="22">
+      <c r="G11" s="22">
         <v>2500</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="H11" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I11" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J11" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L11" s="8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>9</v>
       </c>
@@ -5504,35 +5440,32 @@
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="11">
-        <v>9</v>
-      </c>
-      <c r="E12" s="22" t="s">
+      <c r="D12" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F12" s="22">
+      <c r="E12" s="22">
         <v>10</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H12" s="22">
+      <c r="G12" s="22">
         <v>2500</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="H12" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I12" s="8" t="s">
+        <v>232</v>
+      </c>
       <c r="J12" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L12" s="8" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>10</v>
       </c>
@@ -5542,40 +5475,37 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="11">
-        <v>10</v>
-      </c>
-      <c r="E13" s="22" t="s">
+      <c r="D13" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="F13" s="22">
+      <c r="E13" s="22">
         <v>5</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H13" s="22">
+      <c r="G13" s="22">
         <v>2500</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="H13" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="I13" s="8" t="s">
+        <v>244</v>
+      </c>
       <c r="J13" s="8" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="L13" s="8" t="s">
         <v>245</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B4:B13">
@@ -5583,7 +5513,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L4" r:id="rId1"/>
+    <hyperlink ref="K4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5593,7 +5523,7 @@
           <x14:formula1>
             <xm:f>Constantes!$Q$2:$Q$12</xm:f>
           </x14:formula1>
-          <xm:sqref>J4:J13</xm:sqref>
+          <xm:sqref>I4:I13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5606,35 +5536,36 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" customWidth="1"/>
-    <col min="6" max="6" width="47.5703125" customWidth="1"/>
-    <col min="7" max="9" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" customWidth="1"/>
+    <col min="6" max="8" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="34" t="s">
         <v>188</v>
       </c>
       <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>246</v>
       </c>
+      <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -5644,26 +5575,23 @@
       <c r="C2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>42</v>
+      <c r="D2" s="24" t="s">
+        <v>149</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>149</v>
+      <c r="F2" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>120</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -5674,25 +5602,22 @@
         <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -5702,24 +5627,21 @@
       <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
-        <v>1</v>
+      <c r="D4" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F4" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G4" s="27">
+      <c r="F4" s="27">
         <v>43570</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -5729,24 +5651,21 @@
       <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="11">
-        <v>2</v>
+      <c r="D5" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F5" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G5" s="27">
+      <c r="F5" s="27">
         <v>43570</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -5756,24 +5675,21 @@
       <c r="C6" s="11">
         <v>1</v>
       </c>
-      <c r="D6" s="11">
-        <v>3</v>
+      <c r="D6" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F6" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G6" s="27">
+      <c r="F6" s="27">
         <v>43570</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22" t="s">
+      <c r="G6" s="22"/>
+      <c r="H6" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -5783,24 +5699,21 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="11">
-        <v>4</v>
+      <c r="D7" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F7" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="27">
+      <c r="F7" s="27">
         <v>43570</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22" t="s">
+      <c r="G7" s="22"/>
+      <c r="H7" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>5</v>
       </c>
@@ -5810,24 +5723,21 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="11">
-        <v>5</v>
+      <c r="D8" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F8" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G8" s="27">
+      <c r="F8" s="27">
         <v>43570</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>6</v>
       </c>
@@ -5837,24 +5747,21 @@
       <c r="C9" s="11">
         <v>1</v>
       </c>
-      <c r="D9" s="11">
-        <v>6</v>
+      <c r="D9" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G9" s="27">
+      <c r="F9" s="27">
         <v>43570</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22" t="s">
+      <c r="G9" s="22"/>
+      <c r="H9" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>7</v>
       </c>
@@ -5864,24 +5771,21 @@
       <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="D10" s="11">
-        <v>7</v>
+      <c r="D10" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F10" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G10" s="27">
+      <c r="F10" s="27">
         <v>43570</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22" t="s">
+      <c r="G10" s="22"/>
+      <c r="H10" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>8</v>
       </c>
@@ -5891,24 +5795,21 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="11">
-        <v>8</v>
+      <c r="D11" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F11" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G11" s="27">
+      <c r="F11" s="27">
         <v>43570</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22" t="s">
+      <c r="G11" s="22"/>
+      <c r="H11" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>9</v>
       </c>
@@ -5918,24 +5819,21 @@
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="11">
-        <v>9</v>
+      <c r="D12" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F12" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G12" s="27">
+      <c r="F12" s="27">
         <v>43570</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22" t="s">
+      <c r="G12" s="22"/>
+      <c r="H12" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>10</v>
       </c>
@@ -5945,27 +5843,24 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="11">
-        <v>10</v>
+      <c r="D13" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F13" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G13" s="27">
+      <c r="F13" s="27">
         <v>43570</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22" t="s">
+      <c r="G13" s="22"/>
+      <c r="H13" s="22" t="s">
         <v>250</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:H1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B4:B13">
@@ -5980,7 +5875,7 @@
           <x14:formula1>
             <xm:f>Constantes!$S$2:$S$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I4:I13</xm:sqref>
+          <xm:sqref>H4:H13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7678,7 +7573,7 @@
   </sheetPr>
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add import script for items, milestones, documents
</commit_message>
<xml_diff>
--- a/server/transparencyportal/upload/imports/local_test.xlsx
+++ b/server/transparencyportal/upload/imports/local_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Guides" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="337">
   <si>
     <t>Couleur des entêtes</t>
   </si>
@@ -1039,6 +1039,9 @@
   </si>
   <si>
     <t>cancellationDetails</t>
+  </si>
+  <si>
+    <t>milestone</t>
   </si>
 </sst>
 </file>
@@ -4575,7 +4578,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D1048576"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4946,13 +4949,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>137</v>
+        <v>336</v>
       </c>
       <c r="C12" s="11">
         <v>1</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>186</v>
@@ -5014,7 +5017,7 @@
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B4:B13">
-      <formula1>"planning,tender,award,contract,implementation"</formula1>
+      <formula1>"planning,tender,award,contract,implementation,milestone"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -5044,7 +5047,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -5538,8 +5541,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>